<commit_message>
vault backup: 2025-05-18 22:08:02
</commit_message>
<xml_diff>
--- a/Images/Sheets/Doll_Charactersheet.xlsx
+++ b/Images/Sheets/Doll_Charactersheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="148">
   <si>
     <t>D.0.L.L</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>HP</t>
+  </si>
+  <si>
+    <t>45-7</t>
   </si>
   <si>
     <t>DEATH SAVE</t>
@@ -3323,15 +3326,15 @@
       <c r="B20" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="70">
-        <v>45.0</v>
+      <c r="C20" s="70" t="s">
+        <v>47</v>
       </c>
       <c r="D20" s="15">
         <f>10+(5*(AVERAGE(I17,I13)))</f>
         <v>45</v>
       </c>
       <c r="E20" s="71" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F20" s="72"/>
       <c r="G20" s="1"/>
@@ -3340,7 +3343,7 @@
       <c r="J20" s="74"/>
       <c r="K20" s="1"/>
       <c r="L20" s="42" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M20" s="43" t="s">
         <v>14</v>
@@ -3368,7 +3371,7 @@
       <c r="F21" s="77"/>
       <c r="G21" s="1"/>
       <c r="H21" s="40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I21" s="78">
         <v>4.0</v>
@@ -3378,7 +3381,7 @@
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="80" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M21" s="81" t="s">
         <v>21</v>
@@ -3404,7 +3407,7 @@
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="86" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C22" s="87">
         <v>49.0</v>
@@ -3414,7 +3417,7 @@
         <v>70</v>
       </c>
       <c r="E22" s="88" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F22" s="89"/>
       <c r="G22" s="9"/>
@@ -3450,7 +3453,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="93"/>
       <c r="L23" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
@@ -3479,26 +3482,26 @@
       <c r="J24" s="1"/>
       <c r="K24" s="94"/>
       <c r="L24" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M24" s="21" t="s">
         <v>8</v>
       </c>
       <c r="N24" s="95"/>
       <c r="O24" s="96" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="P24" s="96" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q24" s="96" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R24" s="96" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="S24" s="97" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="T24" s="22"/>
       <c r="U24" s="22"/>
@@ -3510,7 +3513,7 @@
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="98" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C25" s="99">
         <f>170+150-120+180+99-450+120+100</f>
@@ -3518,7 +3521,7 @@
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="100" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F25" s="99">
         <f>100</f>
@@ -3530,7 +3533,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="94"/>
       <c r="L25" s="101" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M25" s="102">
         <f>O5</f>
@@ -3538,7 +3541,7 @@
       </c>
       <c r="N25" s="103"/>
       <c r="O25" s="104" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="P25" s="104">
         <v>2.0</v>
@@ -3550,7 +3553,7 @@
         <v>16</v>
       </c>
       <c r="S25" s="106" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="T25" s="107"/>
       <c r="U25" s="107"/>
@@ -3572,7 +3575,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="94"/>
       <c r="L26" s="110" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M26" s="111">
         <f>O17</f>
@@ -3580,19 +3583,19 @@
       </c>
       <c r="N26" s="112"/>
       <c r="O26" s="113" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="P26" s="113">
         <v>2.0</v>
       </c>
       <c r="Q26" s="114" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R26" s="113" t="s">
         <v>16</v>
       </c>
       <c r="S26" s="115" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="T26" s="116"/>
       <c r="U26" s="116"/>
@@ -3604,7 +3607,7 @@
     <row r="27" ht="18.0" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -3633,17 +3636,17 @@
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="119"/>
       <c r="B28" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C28" s="96"/>
       <c r="D28" s="96" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E28" s="96" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F28" s="97" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G28" s="22"/>
       <c r="H28" s="22"/>
@@ -3668,7 +3671,7 @@
     <row r="29" ht="14.25" customHeight="1">
       <c r="A29" s="119"/>
       <c r="B29" s="120" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C29" s="121"/>
       <c r="D29" s="122">
@@ -3705,13 +3708,13 @@
       </c>
       <c r="C30" s="100"/>
       <c r="D30" s="100" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E30" s="100" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F30" s="100" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G30" s="100"/>
       <c r="H30" s="100"/>
@@ -3736,7 +3739,7 @@
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="119"/>
       <c r="B31" s="126" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C31" s="127"/>
       <c r="D31" s="128">
@@ -3769,17 +3772,17 @@
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="119"/>
       <c r="B32" s="98" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C32" s="100"/>
       <c r="D32" s="100" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E32" s="100" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F32" s="100" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G32" s="100"/>
       <c r="H32" s="100"/>
@@ -3860,7 +3863,7 @@
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="1"/>
       <c r="B35" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -3879,7 +3882,7 @@
       <c r="Q35" s="142"/>
       <c r="R35" s="142"/>
       <c r="S35" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="T35" s="11"/>
       <c r="U35" s="11"/>
@@ -3891,12 +3894,12 @@
     <row r="36" ht="18.0" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="144" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C36" s="22"/>
       <c r="D36" s="145"/>
       <c r="E36" s="146" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
@@ -3904,16 +3907,16 @@
       <c r="I36" s="23"/>
       <c r="J36" s="94"/>
       <c r="K36" s="147" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L36" s="95"/>
       <c r="M36" s="97" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N36" s="22"/>
       <c r="O36" s="95"/>
       <c r="P36" s="21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Q36" s="23"/>
       <c r="R36" s="1"/>
@@ -3932,12 +3935,12 @@
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="148" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="149"/>
       <c r="E37" s="150" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
@@ -3947,12 +3950,12 @@
       <c r="K37" s="152"/>
       <c r="L37" s="103"/>
       <c r="M37" s="153" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N37" s="107"/>
       <c r="O37" s="103"/>
       <c r="P37" s="153" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="Q37" s="108"/>
       <c r="R37" s="1"/>
@@ -3967,12 +3970,12 @@
     <row r="38" ht="14.25" customHeight="1">
       <c r="A38" s="1"/>
       <c r="B38" s="156" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="149"/>
       <c r="E38" s="157" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
@@ -3985,7 +3988,7 @@
       <c r="N38" s="116"/>
       <c r="O38" s="112"/>
       <c r="P38" s="159" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="Q38" s="117"/>
       <c r="R38" s="1"/>
@@ -4000,12 +4003,12 @@
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="1"/>
       <c r="B39" s="148" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="149"/>
       <c r="E39" s="150" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
@@ -4031,12 +4034,12 @@
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="1"/>
       <c r="B40" s="156" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="149"/>
       <c r="E40" s="162" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
@@ -4062,12 +4065,12 @@
     <row r="41" ht="14.25" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="148" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="149"/>
       <c r="E41" s="163" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
@@ -4075,7 +4078,7 @@
       <c r="I41" s="151"/>
       <c r="J41" s="1"/>
       <c r="K41" s="144" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="L41" s="22"/>
       <c r="M41" s="22"/>
@@ -4095,12 +4098,12 @@
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="1"/>
       <c r="B42" s="156" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="149"/>
       <c r="E42" s="157" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
@@ -4108,7 +4111,7 @@
       <c r="I42" s="151"/>
       <c r="J42" s="1"/>
       <c r="K42" s="164" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L42" s="36"/>
       <c r="M42" s="36"/>
@@ -4128,12 +4131,12 @@
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="148" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="149"/>
       <c r="E43" s="150" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
@@ -4154,12 +4157,12 @@
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="156" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C44" s="11"/>
       <c r="D44" s="149"/>
       <c r="E44" s="157" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
@@ -4180,12 +4183,12 @@
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="165" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="166"/>
       <c r="E45" s="167" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
@@ -4211,12 +4214,12 @@
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="144" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C46" s="22"/>
       <c r="D46" s="145"/>
       <c r="E46" s="146" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F46" s="22"/>
       <c r="G46" s="22"/>
@@ -4242,12 +4245,12 @@
     <row r="47" ht="12.75" customHeight="1">
       <c r="A47" s="1"/>
       <c r="B47" s="169" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C47" s="36"/>
       <c r="D47" s="170"/>
       <c r="E47" s="171" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F47" s="36"/>
       <c r="G47" s="36"/>
@@ -4255,7 +4258,7 @@
       <c r="I47" s="37"/>
       <c r="J47" s="1"/>
       <c r="K47" s="172" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L47" s="22"/>
       <c r="M47" s="22"/>
@@ -4280,7 +4283,7 @@
       <c r="I48" s="39"/>
       <c r="J48" s="1"/>
       <c r="K48" s="174" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L48" s="36"/>
       <c r="M48" s="36"/>
@@ -4354,7 +4357,7 @@
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="1"/>
       <c r="B51" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C51" s="11"/>
       <c r="D51" s="11"/>
@@ -4372,7 +4375,7 @@
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
       <c r="R51" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="S51" s="11"/>
       <c r="T51" s="11"/>
@@ -4390,28 +4393,28 @@
       <c r="C52" s="22"/>
       <c r="D52" s="95"/>
       <c r="E52" s="177" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F52" s="22"/>
       <c r="G52" s="95"/>
       <c r="H52" s="177" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I52" s="95"/>
       <c r="J52" s="177" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="K52" s="22"/>
       <c r="L52" s="95"/>
       <c r="M52" s="177" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N52" s="22"/>
       <c r="O52" s="23"/>
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="178" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="S52" s="179"/>
       <c r="T52" s="179"/>
@@ -4424,12 +4427,12 @@
     <row r="53" ht="14.25" customHeight="1">
       <c r="A53" s="1"/>
       <c r="B53" s="181" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C53" s="36"/>
       <c r="D53" s="170"/>
       <c r="E53" s="182" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F53" s="36"/>
       <c r="G53" s="170"/>
@@ -4438,7 +4441,7 @@
       </c>
       <c r="I53" s="170"/>
       <c r="J53" s="184" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K53" s="36"/>
       <c r="L53" s="185"/>
@@ -4450,7 +4453,7 @@
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
       <c r="R53" s="186" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="S53" s="116"/>
       <c r="T53" s="116"/>
@@ -4475,7 +4478,7 @@
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
       <c r="R54" s="186" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S54" s="116"/>
       <c r="T54" s="116"/>
@@ -4504,7 +4507,7 @@
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
       <c r="R55" s="191" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="S55" s="58"/>
       <c r="T55" s="58"/>
@@ -4517,12 +4520,12 @@
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="1"/>
       <c r="B56" s="192" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C56" s="58"/>
       <c r="D56" s="193"/>
       <c r="E56" s="194" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F56" s="58"/>
       <c r="G56" s="193"/>
@@ -4531,7 +4534,7 @@
       </c>
       <c r="I56" s="193"/>
       <c r="J56" s="196" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="K56" s="58"/>
       <c r="L56" s="197"/>
@@ -4566,7 +4569,7 @@
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
       <c r="R57" s="186" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="S57" s="116"/>
       <c r="T57" s="116"/>
@@ -4606,12 +4609,12 @@
     <row r="59" ht="14.25" customHeight="1">
       <c r="A59" s="1"/>
       <c r="B59" s="192" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C59" s="58"/>
       <c r="D59" s="193"/>
       <c r="E59" s="194" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F59" s="58"/>
       <c r="G59" s="193"/>
@@ -4620,12 +4623,12 @@
       </c>
       <c r="I59" s="193"/>
       <c r="J59" s="198" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K59" s="58"/>
       <c r="L59" s="197"/>
       <c r="M59" s="199" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N59" s="58"/>
       <c r="O59" s="59"/>
@@ -4670,12 +4673,12 @@
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="1"/>
       <c r="B61" s="192" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C61" s="58"/>
       <c r="D61" s="193"/>
       <c r="E61" s="194" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F61" s="58"/>
       <c r="G61" s="193"/>
@@ -4684,7 +4687,7 @@
       </c>
       <c r="I61" s="193"/>
       <c r="J61" s="198" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K61" s="58"/>
       <c r="L61" s="197"/>
@@ -4757,12 +4760,12 @@
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="1"/>
       <c r="B64" s="192" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C64" s="58"/>
       <c r="D64" s="193"/>
       <c r="E64" s="194" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F64" s="58"/>
       <c r="G64" s="193"/>
@@ -4771,7 +4774,7 @@
       </c>
       <c r="I64" s="193"/>
       <c r="J64" s="200" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K64" s="58"/>
       <c r="L64" s="193"/>
@@ -4844,12 +4847,12 @@
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="1"/>
       <c r="B67" s="181" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C67" s="36"/>
       <c r="D67" s="170"/>
       <c r="E67" s="182" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F67" s="36"/>
       <c r="G67" s="170"/>
@@ -4858,7 +4861,7 @@
       </c>
       <c r="I67" s="170"/>
       <c r="J67" s="202" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K67" s="36"/>
       <c r="L67" s="185"/>
@@ -5001,7 +5004,7 @@
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="206" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -27538,16 +27541,16 @@
         <v>7</v>
       </c>
       <c r="C1" s="208" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D1" s="209"/>
       <c r="E1" s="209"/>
       <c r="F1" s="209"/>
       <c r="G1" s="208" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="208" t="s">
         <v>137</v>
-      </c>
-      <c r="H1" s="208" t="s">
-        <v>136</v>
       </c>
       <c r="I1" s="209"/>
       <c r="J1" s="209"/>
@@ -27580,7 +27583,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="210" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H2" s="210">
         <v>10.0</v>
@@ -27606,7 +27609,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="210" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H3" s="210">
         <v>10.0</v>
@@ -27624,7 +27627,7 @@
         <v>4</v>
       </c>
       <c r="G4" s="210" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H4" s="210">
         <v>100.0</v>
@@ -27642,7 +27645,7 @@
         <v>6</v>
       </c>
       <c r="G5" s="210" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H5" s="210">
         <v>100.0</v>
@@ -27660,7 +27663,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="210" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H6" s="210">
         <v>100.0</v>
@@ -27678,7 +27681,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="210" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H7" s="210">
         <v>500.0</v>
@@ -27699,7 +27702,7 @@
         <v>2</v>
       </c>
       <c r="G8" s="210" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H8" s="210">
         <v>100.0</v>
@@ -27720,7 +27723,7 @@
         <v>6</v>
       </c>
       <c r="G9" s="210" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H9" s="210">
         <v>100.0</v>
@@ -27741,7 +27744,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="210" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H10" s="210">
         <v>100.0</v>
@@ -27764,7 +27767,7 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="210" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B12" s="210">
         <v>6.0</v>
@@ -27776,7 +27779,7 @@
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="210" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B13" s="210">
         <v>4.0</v>
@@ -27788,7 +27791,7 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="210" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B14" s="210">
         <v>4.0</v>
@@ -27799,7 +27802,7 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="210" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B15" s="210">
         <v>6.0</v>
@@ -27823,7 +27826,7 @@
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="210" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B17" s="210">
         <v>6.0</v>
@@ -27835,7 +27838,7 @@
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="210" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B18" s="210">
         <v>3.0</v>
@@ -27847,7 +27850,7 @@
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="210" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B19" s="210">
         <v>6.0</v>

</xml_diff>

<commit_message>
vault backup: 2025-05-18 22:11:08
</commit_message>
<xml_diff>
--- a/Images/Sheets/Doll_Charactersheet.xlsx
+++ b/Images/Sheets/Doll_Charactersheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="147">
   <si>
     <t>D.0.L.L</t>
   </si>
@@ -258,9 +258,6 @@
   </si>
   <si>
     <t>HP</t>
-  </si>
-  <si>
-    <t>45-7</t>
   </si>
   <si>
     <t>DEATH SAVE</t>
@@ -3326,15 +3323,16 @@
       <c r="B20" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="70" t="s">
-        <v>47</v>
+      <c r="C20" s="70">
+        <f> 45-7-9-7</f>
+        <v>22</v>
       </c>
       <c r="D20" s="15">
         <f>10+(5*(AVERAGE(I17,I13)))</f>
         <v>45</v>
       </c>
       <c r="E20" s="71" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F20" s="72"/>
       <c r="G20" s="1"/>
@@ -3343,7 +3341,7 @@
       <c r="J20" s="74"/>
       <c r="K20" s="1"/>
       <c r="L20" s="42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M20" s="43" t="s">
         <v>14</v>
@@ -3371,7 +3369,7 @@
       <c r="F21" s="77"/>
       <c r="G21" s="1"/>
       <c r="H21" s="40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I21" s="78">
         <v>4.0</v>
@@ -3381,7 +3379,7 @@
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="80" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M21" s="81" t="s">
         <v>21</v>
@@ -3407,7 +3405,7 @@
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="86" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" s="87">
         <v>49.0</v>
@@ -3417,7 +3415,7 @@
         <v>70</v>
       </c>
       <c r="E22" s="88" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F22" s="89"/>
       <c r="G22" s="9"/>
@@ -3453,7 +3451,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="93"/>
       <c r="L23" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
@@ -3482,26 +3480,26 @@
       <c r="J24" s="1"/>
       <c r="K24" s="94"/>
       <c r="L24" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M24" s="21" t="s">
         <v>8</v>
       </c>
       <c r="N24" s="95"/>
       <c r="O24" s="96" t="s">
+        <v>55</v>
+      </c>
+      <c r="P24" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="P24" s="96" t="s">
+      <c r="Q24" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="Q24" s="96" t="s">
+      <c r="R24" s="96" t="s">
         <v>58</v>
       </c>
-      <c r="R24" s="96" t="s">
+      <c r="S24" s="97" t="s">
         <v>59</v>
-      </c>
-      <c r="S24" s="97" t="s">
-        <v>60</v>
       </c>
       <c r="T24" s="22"/>
       <c r="U24" s="22"/>
@@ -3513,7 +3511,7 @@
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="98" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25" s="99">
         <f>170+150-120+180+99-450+120+100</f>
@@ -3521,7 +3519,7 @@
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="100" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F25" s="99">
         <f>100</f>
@@ -3533,7 +3531,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="94"/>
       <c r="L25" s="101" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M25" s="102">
         <f>O5</f>
@@ -3541,7 +3539,7 @@
       </c>
       <c r="N25" s="103"/>
       <c r="O25" s="104" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P25" s="104">
         <v>2.0</v>
@@ -3553,7 +3551,7 @@
         <v>16</v>
       </c>
       <c r="S25" s="106" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T25" s="107"/>
       <c r="U25" s="107"/>
@@ -3575,7 +3573,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="94"/>
       <c r="L26" s="110" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M26" s="111">
         <f>O17</f>
@@ -3583,19 +3581,19 @@
       </c>
       <c r="N26" s="112"/>
       <c r="O26" s="113" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P26" s="113">
         <v>2.0</v>
       </c>
       <c r="Q26" s="114" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R26" s="113" t="s">
         <v>16</v>
       </c>
       <c r="S26" s="115" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="T26" s="116"/>
       <c r="U26" s="116"/>
@@ -3607,7 +3605,7 @@
     <row r="27" ht="18.0" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -3636,17 +3634,17 @@
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="119"/>
       <c r="B28" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C28" s="96"/>
       <c r="D28" s="96" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="96" t="s">
         <v>71</v>
       </c>
-      <c r="E28" s="96" t="s">
-        <v>72</v>
-      </c>
       <c r="F28" s="97" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G28" s="22"/>
       <c r="H28" s="22"/>
@@ -3671,7 +3669,7 @@
     <row r="29" ht="14.25" customHeight="1">
       <c r="A29" s="119"/>
       <c r="B29" s="120" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C29" s="121"/>
       <c r="D29" s="122">
@@ -3708,13 +3706,13 @@
       </c>
       <c r="C30" s="100"/>
       <c r="D30" s="100" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="100" t="s">
         <v>71</v>
       </c>
-      <c r="E30" s="100" t="s">
-        <v>72</v>
-      </c>
       <c r="F30" s="100" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G30" s="100"/>
       <c r="H30" s="100"/>
@@ -3739,11 +3737,11 @@
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="119"/>
       <c r="B31" s="126" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C31" s="127"/>
       <c r="D31" s="128">
-        <v>10.0</v>
+        <v>7.0</v>
       </c>
       <c r="E31" s="123" t="s">
         <v>16</v>
@@ -3772,17 +3770,17 @@
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="119"/>
       <c r="B32" s="98" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C32" s="100"/>
       <c r="D32" s="100" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" s="100" t="s">
         <v>71</v>
       </c>
-      <c r="E32" s="100" t="s">
-        <v>72</v>
-      </c>
       <c r="F32" s="100" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G32" s="100"/>
       <c r="H32" s="100"/>
@@ -3863,7 +3861,7 @@
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="1"/>
       <c r="B35" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -3882,7 +3880,7 @@
       <c r="Q35" s="142"/>
       <c r="R35" s="142"/>
       <c r="S35" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T35" s="11"/>
       <c r="U35" s="11"/>
@@ -3894,12 +3892,12 @@
     <row r="36" ht="18.0" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="144" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36" s="22"/>
       <c r="D36" s="145"/>
       <c r="E36" s="146" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
@@ -3907,16 +3905,16 @@
       <c r="I36" s="23"/>
       <c r="J36" s="94"/>
       <c r="K36" s="147" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L36" s="95"/>
       <c r="M36" s="97" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N36" s="22"/>
       <c r="O36" s="95"/>
       <c r="P36" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q36" s="23"/>
       <c r="R36" s="1"/>
@@ -3935,12 +3933,12 @@
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="148" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="149"/>
       <c r="E37" s="150" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
@@ -3950,12 +3948,12 @@
       <c r="K37" s="152"/>
       <c r="L37" s="103"/>
       <c r="M37" s="153" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N37" s="107"/>
       <c r="O37" s="103"/>
       <c r="P37" s="153" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q37" s="108"/>
       <c r="R37" s="1"/>
@@ -3970,12 +3968,12 @@
     <row r="38" ht="14.25" customHeight="1">
       <c r="A38" s="1"/>
       <c r="B38" s="156" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="149"/>
       <c r="E38" s="157" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
@@ -3988,7 +3986,7 @@
       <c r="N38" s="116"/>
       <c r="O38" s="112"/>
       <c r="P38" s="159" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q38" s="117"/>
       <c r="R38" s="1"/>
@@ -4003,12 +4001,12 @@
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="1"/>
       <c r="B39" s="148" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="149"/>
       <c r="E39" s="150" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
@@ -4034,12 +4032,12 @@
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="1"/>
       <c r="B40" s="156" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="149"/>
       <c r="E40" s="162" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
@@ -4065,12 +4063,12 @@
     <row r="41" ht="14.25" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="148" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="149"/>
       <c r="E41" s="163" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
@@ -4078,7 +4076,7 @@
       <c r="I41" s="151"/>
       <c r="J41" s="1"/>
       <c r="K41" s="144" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L41" s="22"/>
       <c r="M41" s="22"/>
@@ -4098,12 +4096,12 @@
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="1"/>
       <c r="B42" s="156" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="149"/>
       <c r="E42" s="157" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
@@ -4111,7 +4109,7 @@
       <c r="I42" s="151"/>
       <c r="J42" s="1"/>
       <c r="K42" s="164" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L42" s="36"/>
       <c r="M42" s="36"/>
@@ -4131,12 +4129,12 @@
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="148" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="149"/>
       <c r="E43" s="150" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
@@ -4157,12 +4155,12 @@
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="156" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C44" s="11"/>
       <c r="D44" s="149"/>
       <c r="E44" s="157" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
@@ -4183,12 +4181,12 @@
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="165" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="166"/>
       <c r="E45" s="167" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
@@ -4214,12 +4212,12 @@
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="144" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C46" s="22"/>
       <c r="D46" s="145"/>
       <c r="E46" s="146" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F46" s="22"/>
       <c r="G46" s="22"/>
@@ -4245,12 +4243,12 @@
     <row r="47" ht="12.75" customHeight="1">
       <c r="A47" s="1"/>
       <c r="B47" s="169" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C47" s="36"/>
       <c r="D47" s="170"/>
       <c r="E47" s="171" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F47" s="36"/>
       <c r="G47" s="36"/>
@@ -4258,7 +4256,7 @@
       <c r="I47" s="37"/>
       <c r="J47" s="1"/>
       <c r="K47" s="172" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L47" s="22"/>
       <c r="M47" s="22"/>
@@ -4283,7 +4281,7 @@
       <c r="I48" s="39"/>
       <c r="J48" s="1"/>
       <c r="K48" s="174" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L48" s="36"/>
       <c r="M48" s="36"/>
@@ -4357,7 +4355,7 @@
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="1"/>
       <c r="B51" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C51" s="11"/>
       <c r="D51" s="11"/>
@@ -4375,7 +4373,7 @@
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
       <c r="R51" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S51" s="11"/>
       <c r="T51" s="11"/>
@@ -4393,28 +4391,28 @@
       <c r="C52" s="22"/>
       <c r="D52" s="95"/>
       <c r="E52" s="177" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F52" s="22"/>
       <c r="G52" s="95"/>
       <c r="H52" s="177" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I52" s="95"/>
       <c r="J52" s="177" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K52" s="22"/>
       <c r="L52" s="95"/>
       <c r="M52" s="177" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N52" s="22"/>
       <c r="O52" s="23"/>
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="178" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S52" s="179"/>
       <c r="T52" s="179"/>
@@ -4427,12 +4425,12 @@
     <row r="53" ht="14.25" customHeight="1">
       <c r="A53" s="1"/>
       <c r="B53" s="181" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C53" s="36"/>
       <c r="D53" s="170"/>
       <c r="E53" s="182" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F53" s="36"/>
       <c r="G53" s="170"/>
@@ -4441,7 +4439,7 @@
       </c>
       <c r="I53" s="170"/>
       <c r="J53" s="184" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K53" s="36"/>
       <c r="L53" s="185"/>
@@ -4453,7 +4451,7 @@
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
       <c r="R53" s="186" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="S53" s="116"/>
       <c r="T53" s="116"/>
@@ -4478,7 +4476,7 @@
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
       <c r="R54" s="186" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="S54" s="116"/>
       <c r="T54" s="116"/>
@@ -4507,7 +4505,7 @@
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
       <c r="R55" s="191" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="S55" s="58"/>
       <c r="T55" s="58"/>
@@ -4520,12 +4518,12 @@
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="1"/>
       <c r="B56" s="192" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C56" s="58"/>
       <c r="D56" s="193"/>
       <c r="E56" s="194" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F56" s="58"/>
       <c r="G56" s="193"/>
@@ -4534,7 +4532,7 @@
       </c>
       <c r="I56" s="193"/>
       <c r="J56" s="196" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K56" s="58"/>
       <c r="L56" s="197"/>
@@ -4569,7 +4567,7 @@
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
       <c r="R57" s="186" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="S57" s="116"/>
       <c r="T57" s="116"/>
@@ -4609,12 +4607,12 @@
     <row r="59" ht="14.25" customHeight="1">
       <c r="A59" s="1"/>
       <c r="B59" s="192" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C59" s="58"/>
       <c r="D59" s="193"/>
       <c r="E59" s="194" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F59" s="58"/>
       <c r="G59" s="193"/>
@@ -4623,12 +4621,12 @@
       </c>
       <c r="I59" s="193"/>
       <c r="J59" s="198" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K59" s="58"/>
       <c r="L59" s="197"/>
       <c r="M59" s="199" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N59" s="58"/>
       <c r="O59" s="59"/>
@@ -4673,12 +4671,12 @@
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="1"/>
       <c r="B61" s="192" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C61" s="58"/>
       <c r="D61" s="193"/>
       <c r="E61" s="194" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F61" s="58"/>
       <c r="G61" s="193"/>
@@ -4687,7 +4685,7 @@
       </c>
       <c r="I61" s="193"/>
       <c r="J61" s="198" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K61" s="58"/>
       <c r="L61" s="197"/>
@@ -4760,12 +4758,12 @@
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="1"/>
       <c r="B64" s="192" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C64" s="58"/>
       <c r="D64" s="193"/>
       <c r="E64" s="194" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F64" s="58"/>
       <c r="G64" s="193"/>
@@ -4774,7 +4772,7 @@
       </c>
       <c r="I64" s="193"/>
       <c r="J64" s="200" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K64" s="58"/>
       <c r="L64" s="193"/>
@@ -4847,12 +4845,12 @@
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="1"/>
       <c r="B67" s="181" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C67" s="36"/>
       <c r="D67" s="170"/>
       <c r="E67" s="182" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F67" s="36"/>
       <c r="G67" s="170"/>
@@ -4861,7 +4859,7 @@
       </c>
       <c r="I67" s="170"/>
       <c r="J67" s="202" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K67" s="36"/>
       <c r="L67" s="185"/>
@@ -5004,7 +5002,7 @@
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="206" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -27541,16 +27539,16 @@
         <v>7</v>
       </c>
       <c r="C1" s="208" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D1" s="209"/>
       <c r="E1" s="209"/>
       <c r="F1" s="209"/>
       <c r="G1" s="208" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H1" s="208" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I1" s="209"/>
       <c r="J1" s="209"/>
@@ -27583,7 +27581,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="210" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H2" s="210">
         <v>10.0</v>
@@ -27609,7 +27607,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="210" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H3" s="210">
         <v>10.0</v>
@@ -27627,7 +27625,7 @@
         <v>4</v>
       </c>
       <c r="G4" s="210" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H4" s="210">
         <v>100.0</v>
@@ -27645,7 +27643,7 @@
         <v>6</v>
       </c>
       <c r="G5" s="210" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H5" s="210">
         <v>100.0</v>
@@ -27663,7 +27661,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="210" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H6" s="210">
         <v>100.0</v>
@@ -27681,7 +27679,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="210" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H7" s="210">
         <v>500.0</v>
@@ -27702,7 +27700,7 @@
         <v>2</v>
       </c>
       <c r="G8" s="210" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H8" s="210">
         <v>100.0</v>
@@ -27723,7 +27721,7 @@
         <v>6</v>
       </c>
       <c r="G9" s="210" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H9" s="210">
         <v>100.0</v>
@@ -27744,7 +27742,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="210" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H10" s="210">
         <v>100.0</v>
@@ -27767,7 +27765,7 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="210" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B12" s="210">
         <v>6.0</v>
@@ -27779,7 +27777,7 @@
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="210" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B13" s="210">
         <v>4.0</v>
@@ -27791,7 +27789,7 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="210" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B14" s="210">
         <v>4.0</v>
@@ -27802,7 +27800,7 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="210" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="210">
         <v>6.0</v>
@@ -27826,7 +27824,7 @@
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="210" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B17" s="210">
         <v>6.0</v>
@@ -27838,7 +27836,7 @@
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="210" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" s="210">
         <v>3.0</v>
@@ -27850,7 +27848,7 @@
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="210" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="210">
         <v>6.0</v>

</xml_diff>

<commit_message>
vault backup: 2025-05-18 22:22:49
</commit_message>
<xml_diff>
--- a/Images/Sheets/Doll_Charactersheet.xlsx
+++ b/Images/Sheets/Doll_Charactersheet.xlsx
@@ -3324,8 +3324,8 @@
         <v>46</v>
       </c>
       <c r="C20" s="70">
-        <f> 45-7-9-7</f>
-        <v>22</v>
+        <f> 45-7-9-7-16</f>
+        <v>6</v>
       </c>
       <c r="D20" s="15">
         <f>10+(5*(AVERAGE(I17,I13)))</f>

</xml_diff>